<commit_message>
AUTO FROM work 06.05.2024 15:02:17,49
</commit_message>
<xml_diff>
--- a/Листопадова/Книга1.xlsx
+++ b/Листопадова/Книга1.xlsx
@@ -822,7 +822,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -853,15 +853,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -869,12 +860,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -1057,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1117,10 +1114,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1425,7 +1433,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,7 +1468,10 @@
       <c r="H1" s="11">
         <v>11.51</v>
       </c>
-      <c r="I1" s="11"/>
+      <c r="I1" s="26">
+        <f>0.39*(89.64*0.4+0.31*0.35)</f>
+        <v>14.026155000000001</v>
+      </c>
       <c r="J1" s="22">
         <v>10</v>
       </c>
@@ -1491,7 +1502,7 @@
       <c r="E2" s="10">
         <v>277.75</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>401.02</v>
       </c>
       <c r="G2">
@@ -1510,7 +1521,9 @@
       </c>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="N2" s="27">
+        <v>49.55</v>
+      </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="13"/>
@@ -1547,12 +1560,14 @@
       <c r="K3" s="13"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="N3" s="28">
+        <v>706.26</v>
+      </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="1:17" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="48" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -1579,12 +1594,22 @@
       <c r="H4" s="11">
         <v>47.03</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="11"/>
+      <c r="I4" s="26">
+        <f xml:space="preserve"> 35.52 + 14.03</f>
+        <v>49.550000000000004</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23">
+        <v>3341.8</v>
+      </c>
+      <c r="L4" s="26">
+        <f xml:space="preserve"> 49.55+ 706.26+240.13+5.52+2354.21</f>
+        <v>3355.67</v>
+      </c>
       <c r="M4" s="11"/>
-      <c r="N4" s="23"/>
+      <c r="N4" s="28">
+        <v>240.13</v>
+      </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="13"/>
@@ -1618,10 +1643,17 @@
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="11"/>
+      <c r="K5" s="13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L5" s="11">
+        <f>89.95/1854.72</f>
+        <v>4.8497886473429952E-2</v>
+      </c>
       <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="28">
+        <v>5.52</v>
+      </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="13"/>
@@ -1653,12 +1685,16 @@
       <c r="H6">
         <v>89.640000000000015</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="24">
+        <v>89.95</v>
+      </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="N6" s="28">
+        <v>2354.21</v>
+      </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="13"/>
@@ -1692,10 +1728,20 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="K7" s="11">
+        <v>4491.3999999999996</v>
+      </c>
+      <c r="L7" s="26">
+        <f xml:space="preserve"> 3758.4+751.68</f>
+        <v>4510.08</v>
+      </c>
+      <c r="M7" s="11">
+        <v>3341.8</v>
+      </c>
+      <c r="N7" s="24">
+        <f>SUM(N2:N6)</f>
+        <v>3355.67</v>
+      </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -1729,11 +1775,19 @@
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
+      <c r="K8" s="11">
+        <v>401.02</v>
+      </c>
+      <c r="L8" s="29">
+        <f>12*3355.67/100</f>
+        <v>402.68040000000002</v>
+      </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="O8" s="11">
+        <f>L8/L7</f>
+        <v>8.9284535972754375E-2</v>
+      </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
     </row>
@@ -1764,13 +1818,23 @@
       <c r="H9" s="22">
         <v>617.4</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="25">
+        <v>619.53</v>
+      </c>
       <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="K9" s="22">
+        <v>3742.82</v>
+      </c>
+      <c r="L9" s="26">
+        <f xml:space="preserve"> 3355.67 + 402.68</f>
+        <v>3758.35</v>
+      </c>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="11">
+        <f>14.03/4510.1</f>
+        <v>3.1107957694951329E-3</v>
+      </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
     </row>
@@ -1801,13 +1865,23 @@
       <c r="H10" s="22">
         <v>703.83</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="24">
+        <v>706.26</v>
+      </c>
       <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="K10" s="22">
+        <v>748.56</v>
+      </c>
+      <c r="L10" s="11">
+        <f>20/100*3758.4</f>
+        <v>751.68000000000006</v>
+      </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="O10" s="11">
+        <f>L4/L7</f>
+        <v>0.74403779977295303</v>
+      </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
     </row>
@@ -1838,7 +1912,9 @@
       <c r="H11" s="22">
         <v>239.3</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="24">
+        <v>240.13</v>
+      </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -1875,7 +1951,10 @@
       <c r="H12" s="22">
         <v>2346.12</v>
       </c>
-      <c r="I12" s="11"/>
+      <c r="I12" s="24">
+        <f>380*I9/100</f>
+        <v>2354.2139999999999</v>
+      </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>

</xml_diff>